<commit_message>
Test cases and Pom pages added
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -5,20 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nandankumar M S\Desktop\JavaPrograms\com.learningMaven\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nandankumar M S\git\DemoWebShop_Selenium\com.learningMaven\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECE89B9-6B1E-4B70-8AFD-6A1E48FA63FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A349D81D-46AF-45B1-938E-61D013662105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Address" sheetId="6" r:id="rId1"/>
     <sheet name="Login" sheetId="7" r:id="rId2"/>
-    <sheet name="Place" sheetId="5" r:id="rId3"/>
-    <sheet name="Register" sheetId="2" r:id="rId4"/>
-    <sheet name="SearchBox" sheetId="3" r:id="rId5"/>
-    <sheet name="Subscribe" sheetId="4" r:id="rId6"/>
+    <sheet name="CountryAndState" sheetId="8" r:id="rId3"/>
+    <sheet name="Place" sheetId="5" r:id="rId4"/>
+    <sheet name="Register" sheetId="2" r:id="rId5"/>
+    <sheet name="SearchBox" sheetId="3" r:id="rId6"/>
+    <sheet name="Subscribe" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t>Nandankumar</t>
   </si>
@@ -168,6 +169,15 @@
   </si>
   <si>
     <t>nandanms@gmail.com</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Texas</t>
   </si>
 </sst>
 </file>
@@ -644,11 +654,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210D4155-AFCA-408D-8D6A-7A56F40861F7}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -676,6 +690,40 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7603B4CF-D60A-4A88-841C-3461E1414E76}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADA3A3F3-C183-43C4-B791-442EC171D543}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -710,7 +758,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A737A6-F418-4B6D-A877-E1481F35AB07}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -830,7 +878,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12102790-D576-4C0D-A7F9-313DB8162D37}">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -865,7 +913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB1F403-EF29-4C86-B93C-16CD8B19E858}">
   <dimension ref="A1:A4"/>
   <sheetViews>

</xml_diff>